<commit_message>
Added the requirements and the method toString()
</commit_message>
<xml_diff>
--- a/docs/Requerimientos y trazabilidad.xlsx
+++ b/docs/Requerimientos y trazabilidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thetr\Documents\Segundo Semestre\APO II\ECLIPSE\Workspace\volleyball-cup\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9C4F3AE-6AF9-4ED9-9B69-75BAB9ACF81B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8890D8FD-0269-4202-8417-54CA788CB098}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9204" xr2:uid="{D01F522C-CD57-4B31-8EB4-CE645565B958}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
   <si>
     <t>Requerimiento</t>
   </si>
@@ -65,29 +65,137 @@
     <t>R6</t>
   </si>
   <si>
-    <t>R7</t>
-  </si>
-  <si>
-    <t>R8</t>
-  </si>
-  <si>
-    <t>R9</t>
-  </si>
-  <si>
-    <t>R10</t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t>R12</t>
+    <t>Leer archivo de texto</t>
+  </si>
+  <si>
+    <t>Ruta del archivo</t>
+  </si>
+  <si>
+    <t>Cargar información</t>
+  </si>
+  <si>
+    <t>Todos los atributos del espectador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agregar a una lista </t>
+  </si>
+  <si>
+    <t>Permite cargar 50% de los espectadores en una lista doblemente enlazada circular. Estos serán considerados participantes.</t>
+  </si>
+  <si>
+    <t>Todos los atributos del participante</t>
+  </si>
+  <si>
+    <t>Búsqueda de espectador</t>
+  </si>
+  <si>
+    <t>Id del espectador</t>
+  </si>
+  <si>
+    <t>Búsqueda de participante</t>
+  </si>
+  <si>
+    <t>Id del participante</t>
+  </si>
+  <si>
+    <t>Permite cargar la información leída del archivo de texto en un árbol binario.</t>
+  </si>
+  <si>
+    <t>Permite la lectura de un archivo de texto con la información de los asistentes (espectadores y posibles participantes).</t>
+  </si>
+  <si>
+    <t>Permite buscar un espectador en el árbol binario por medio de su id. También devuelve el tiempo que se tardó el programa realizando la búsqueda.</t>
+  </si>
+  <si>
+    <t>Permite buscar un participante en la lista por medio de su id. También devuelve el tiempo que se tardó el programa realizando la búsqueda.</t>
+  </si>
+  <si>
+    <t>Retorna todos los datos del participante encontrado o, en caso de no encontrarse, un mensaje informandole al usuario.</t>
+  </si>
+  <si>
+    <t>Retorna todos los datos del espectador encontrado o, en caso de no encontrarse, un mensaje informandole al usuario.</t>
+  </si>
+  <si>
+    <t>Se crea y agrega cada participante a la lista correctamente.</t>
+  </si>
+  <si>
+    <t>Se crea y agrega cada espectador al árbol binario correctamente.</t>
+  </si>
+  <si>
+    <t>Se lee el archivo de texto con la información correctamente.</t>
+  </si>
+  <si>
+    <t>Visualizar estructuras por país</t>
+  </si>
+  <si>
+    <t xml:space="preserve">País del que se desea visualizar la estructura </t>
+  </si>
+  <si>
+    <t>Permite visualizar ambas estructuras, especatores y participantes (árbol binario y lista enlazada) por separado. La estructura mostrada será de un país específico.</t>
+  </si>
+  <si>
+    <t>Se muestra la estructura deseada de su respectivo país.</t>
+  </si>
+  <si>
+    <t>Requerimientos Funcionales</t>
+  </si>
+  <si>
+    <t>Trazabilidad</t>
+  </si>
+  <si>
+    <t>Clase</t>
+  </si>
+  <si>
+    <t>Método</t>
+  </si>
+  <si>
+    <t>loadInfo(String)</t>
+  </si>
+  <si>
+    <t>addSpectator(String, String, String, String, String, String, String, String)</t>
+  </si>
+  <si>
+    <t>exploreFile(ActionEvent)</t>
+  </si>
+  <si>
+    <t>loadFile(ActionEvent)</t>
+  </si>
+  <si>
+    <t>addParticipant(String, String, String, String, String, String, String, String)</t>
+  </si>
+  <si>
+    <t>searchSpectator(ActionEvent)</t>
+  </si>
+  <si>
+    <t>searchingSpectator(String)</t>
+  </si>
+  <si>
+    <t>searchingParticipant(String)</t>
+  </si>
+  <si>
+    <t>searchParticipant(ActionEvent)</t>
+  </si>
+  <si>
+    <t>VolleyballCup</t>
+  </si>
+  <si>
+    <t>VolleyController</t>
+  </si>
+  <si>
+    <t>CompareTo(Spectator)</t>
+  </si>
+  <si>
+    <t>Spectator</t>
+  </si>
+  <si>
+    <t>createCountryList(String)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,19 +203,151 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -116,9 +356,91 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -435,168 +757,338 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C654AF1-D328-4FCA-9C02-B2147883C250}">
-  <dimension ref="C3:G18"/>
+  <dimension ref="C1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="37.33203125" customWidth="1"/>
+    <col min="5" max="5" width="42.109375" customWidth="1"/>
     <col min="6" max="6" width="28.44140625" customWidth="1"/>
     <col min="7" max="7" width="38.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C3" s="1" t="s">
+    <row r="1" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C4" s="1" t="s">
+    <row r="4" spans="3:7" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C5" s="1" t="s">
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C6" s="1" t="s">
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C7" s="1" t="s">
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" ht="58.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C8" s="1" t="s">
+      <c r="D7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" ht="58.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C9" s="1" t="s">
+      <c r="D8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" ht="58.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C10" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="D9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+    <row r="11" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="27"/>
+      <c r="E11" s="28"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+    <row r="12" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>38</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+    <row r="13" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+    <row r="14" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="7"/>
+      <c r="D14" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>41</v>
+      </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+    <row r="15" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="7"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="9" t="s">
+        <v>42</v>
+      </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+    <row r="16" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+    <row r="17" spans="3:7" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="7"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+    <row r="18" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="7"/>
+      <c r="D18" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>50</v>
+      </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
+    <row r="19" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="11"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="14"/>
+      <c r="D22" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="11"/>
+      <c r="D23" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C24" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="11"/>
+      <c r="D25" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="C16:C18"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added a couple of requirements, some tests, and the visible list of participants
</commit_message>
<xml_diff>
--- a/docs/Requerimientos y trazabilidad.xlsx
+++ b/docs/Requerimientos y trazabilidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thetr\Documents\Segundo Semestre\APO II\ECLIPSE\Workspace\volleyball-cup\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8890D8FD-0269-4202-8417-54CA788CB098}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21C0FA2-16CF-43D2-B4DA-7DE45D845A63}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9204" xr2:uid="{D01F522C-CD57-4B31-8EB4-CE645565B958}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="65">
   <si>
     <t>Requerimiento</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Ruta del archivo</t>
   </si>
   <si>
-    <t>Cargar información</t>
-  </si>
-  <si>
     <t>Todos los atributos del espectador</t>
   </si>
   <si>
@@ -104,12 +101,6 @@
     <t>Permite la lectura de un archivo de texto con la información de los asistentes (espectadores y posibles participantes).</t>
   </si>
   <si>
-    <t>Permite buscar un espectador en el árbol binario por medio de su id. También devuelve el tiempo que se tardó el programa realizando la búsqueda.</t>
-  </si>
-  <si>
-    <t>Permite buscar un participante en la lista por medio de su id. También devuelve el tiempo que se tardó el programa realizando la búsqueda.</t>
-  </si>
-  <si>
     <t>Retorna todos los datos del participante encontrado o, en caso de no encontrarse, un mensaje informandole al usuario.</t>
   </si>
   <si>
@@ -125,18 +116,6 @@
     <t>Se lee el archivo de texto con la información correctamente.</t>
   </si>
   <si>
-    <t>Visualizar estructuras por país</t>
-  </si>
-  <si>
-    <t xml:space="preserve">País del que se desea visualizar la estructura </t>
-  </si>
-  <si>
-    <t>Permite visualizar ambas estructuras, especatores y participantes (árbol binario y lista enlazada) por separado. La estructura mostrada será de un país específico.</t>
-  </si>
-  <si>
-    <t>Se muestra la estructura deseada de su respectivo país.</t>
-  </si>
-  <si>
     <t>Requerimientos Funcionales</t>
   </si>
   <si>
@@ -189,6 +168,63 @@
   </si>
   <si>
     <t>createCountryList(String)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Permite buscar un espectador en el árbol binario por medio de su id. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Permite buscar un participante en la lista por medio de su id. </t>
+  </si>
+  <si>
+    <t>Permite mostrar el tiempo que se tardó en programa en realizar una acción determinada (Buscar espectadores y buscar participantes).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visualizar tiempo </t>
+  </si>
+  <si>
+    <t>Cargar información y agregar a un árbol</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>Mostrar espectadores de un país</t>
+  </si>
+  <si>
+    <t>Permite al usuario elegir un país del cual quiera ver su estructura de espectadores (árbol binario).</t>
+  </si>
+  <si>
+    <t>País</t>
+  </si>
+  <si>
+    <t>Se muestra un diagrama de la estructura por espectadores del país escogido.</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>Mostrar participantes de un país</t>
+  </si>
+  <si>
+    <t>Permite al usuario elegir un país del cual quiera ver su estructura de participantes (lista enlazada).</t>
+  </si>
+  <si>
+    <t>Se muestra un diagrama de la estructura por participantes del país escogido.</t>
+  </si>
+  <si>
+    <t>Se muestra el tiempo (en segundos) que se tardó el programa en realizar dicha acción, ya sea si logró encontrar lo que se buscaba o no.</t>
+  </si>
+  <si>
+    <t>createSpectatorTree(String, String)</t>
+  </si>
+  <si>
+    <t>loadCountry(ActionEvent)</t>
+  </si>
+  <si>
+    <t>showSpectators(ActionEvent)</t>
+  </si>
+  <si>
+    <t>showParticipants(ActionEvent)</t>
   </si>
 </sst>
 </file>
@@ -211,7 +247,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -232,25 +268,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -356,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -367,6 +391,30 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -376,45 +424,32 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -422,26 +457,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -757,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C654AF1-D328-4FCA-9C02-B2147883C250}">
-  <dimension ref="C1:G27"/>
+  <dimension ref="C1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -774,13 +797,13 @@
   <sheetData>
     <row r="1" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6"/>
+      <c r="C2" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" s="3" t="s">
@@ -807,13 +830,13 @@
         <v>11</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="3:7" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -821,16 +844,16 @@
         <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="G5" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="3:7" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -838,50 +861,50 @@
         <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="G6" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7" ht="58.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="3:7" ht="58.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="3:7" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="3:7" ht="58.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -889,204 +912,309 @@
         <v>10</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>32</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="F9" s="2"/>
       <c r="G9" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="29" t="s">
-        <v>38</v>
-      </c>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C13" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>39</v>
-      </c>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.3">
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="7"/>
-      <c r="D14" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>41</v>
-      </c>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.3">
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="7"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="9" t="s">
-        <v>42</v>
-      </c>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.3">
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C16" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>39</v>
-      </c>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.3">
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="3:7" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="7"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="2" t="s">
-        <v>40</v>
-      </c>
+    <row r="17" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="7"/>
-      <c r="D18" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>50</v>
-      </c>
+      <c r="C18" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="16"/>
+      <c r="E18" s="17"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="21"/>
+      <c r="D21" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="22"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C24" s="21"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="22"/>
+      <c r="D25" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="8" t="s">
+      <c r="D26" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C27" s="10"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C28" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C29" s="11"/>
+      <c r="D29" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C30" s="10"/>
+      <c r="D30" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C31" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="3:7" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="11"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C21" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" s="8" t="s">
+    <row r="32" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C32" s="10"/>
+      <c r="D32" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C33" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C35" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C36" s="19"/>
+      <c r="D36" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C38" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E38" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="14"/>
-      <c r="D22" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C23" s="11"/>
-      <c r="D23" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C24" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C25" s="11"/>
-      <c r="D25" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C26" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="3:7" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C39" s="11"/>
+      <c r="D39" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C40" s="10"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D19:D20"/>
+  <mergeCells count="16">
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="D39:D40"/>
     <mergeCell ref="C2:G2"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="D21:D22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>